<commit_message>
finished adding bold in best results
</commit_message>
<xml_diff>
--- a/results_analysis/spark_wallFollow_01_hold_02_best.xlsx
+++ b/results_analysis/spark_wallFollow_01_hold_02_best.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB59772A-C85E-4AF9-A47C-213F3BD24D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AAE62B-379B-4438-B8F9-CF038C8890DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -1689,6 +1689,30 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1714,30 +1738,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2022,8 +2022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2044,35 +2044,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="77" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -2679,7 +2679,7 @@
       <c r="D23" s="60">
         <v>0.453482378854626</v>
       </c>
-      <c r="E23" s="77">
+      <c r="E23" s="68">
         <v>0.93337004405286295</v>
       </c>
       <c r="F23" s="61">
@@ -2688,7 +2688,7 @@
       <c r="G23" s="61">
         <v>0.92945594713656399</v>
       </c>
-      <c r="H23" s="77">
+      <c r="H23" s="68">
         <v>0.93913876651982398</v>
       </c>
       <c r="I23" s="61">
@@ -2697,7 +2697,7 @@
       <c r="J23" s="61">
         <v>0.57376651982378901</v>
       </c>
-      <c r="K23" s="78">
+      <c r="K23" s="69">
         <v>0.93748017621145396</v>
       </c>
     </row>
@@ -2709,19 +2709,19 @@
       <c r="D24" s="63">
         <v>0.73518942731277503</v>
       </c>
-      <c r="E24" s="79">
+      <c r="E24" s="70">
         <v>0.95305286343612305</v>
       </c>
       <c r="F24" s="64">
         <v>0.87319162995594701</v>
       </c>
-      <c r="G24" s="79">
+      <c r="G24" s="70">
         <v>0.95305286343612405</v>
       </c>
-      <c r="H24" s="79">
+      <c r="H24" s="70">
         <v>0.95208149779735696</v>
       </c>
-      <c r="I24" s="64">
+      <c r="I24" s="70">
         <v>0.96028854625550697</v>
       </c>
       <c r="J24" s="64">
@@ -2742,19 +2742,19 @@
       <c r="D25" s="60">
         <v>0.934522026431718</v>
       </c>
-      <c r="E25" s="77">
+      <c r="E25" s="68">
         <v>0.94374229074889904</v>
       </c>
       <c r="F25" s="61">
         <v>0.93118061674008801</v>
       </c>
-      <c r="G25" s="77">
+      <c r="G25" s="68">
         <v>0.94810352422907496</v>
       </c>
       <c r="H25" s="61">
         <v>0.93842511013215901</v>
       </c>
-      <c r="I25" s="77">
+      <c r="I25" s="68">
         <v>0.962834801762114</v>
       </c>
       <c r="J25" s="61">
@@ -2775,7 +2775,7 @@
       <c r="E26" s="64">
         <v>0.95241629955947205</v>
       </c>
-      <c r="F26" s="79">
+      <c r="F26" s="70">
         <v>0.95741189427312801</v>
       </c>
       <c r="G26" s="64">
@@ -2784,13 +2784,13 @@
       <c r="H26" s="64">
         <v>0.95100660792951597</v>
       </c>
-      <c r="I26" s="79">
+      <c r="I26" s="70">
         <v>0.96252863436123404</v>
       </c>
-      <c r="J26" s="79">
+      <c r="J26" s="70">
         <v>0.95514977973568305</v>
       </c>
-      <c r="K26" s="80">
+      <c r="K26" s="71">
         <v>0.960123348017621</v>
       </c>
     </row>
@@ -2802,28 +2802,28 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="81">
+      <c r="D27" s="72">
         <v>0.94958590308369994</v>
       </c>
-      <c r="E27" s="77">
+      <c r="E27" s="68">
         <v>0.95138766519823803</v>
       </c>
-      <c r="F27" s="77">
+      <c r="F27" s="68">
         <v>0.95185242290748895</v>
       </c>
-      <c r="G27" s="77">
+      <c r="G27" s="68">
         <v>0.95113876651982399</v>
       </c>
-      <c r="H27" s="77">
+      <c r="H27" s="68">
         <v>0.95166299559471401</v>
       </c>
-      <c r="I27" s="77">
+      <c r="I27" s="68">
         <v>0.95348898678414096</v>
       </c>
       <c r="J27" s="61">
         <v>0.91534361233480199</v>
       </c>
-      <c r="K27" s="78">
+      <c r="K27" s="69">
         <v>0.95140528634361199</v>
       </c>
     </row>
@@ -2833,7 +2833,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="82">
+      <c r="D28" s="73">
         <v>0.75278634361233498</v>
       </c>
       <c r="E28" s="64">
@@ -2842,13 +2842,13 @@
       <c r="F28" s="64">
         <v>0.74117400881057305</v>
       </c>
-      <c r="G28" s="79">
+      <c r="G28" s="70">
         <v>0.949656387665198</v>
       </c>
       <c r="H28" s="64">
         <v>0.64203524229074904</v>
       </c>
-      <c r="I28" s="79">
+      <c r="I28" s="70">
         <v>0.95284801762114502</v>
       </c>
       <c r="J28" s="64">
@@ -2869,25 +2869,25 @@
       <c r="D29" s="66">
         <v>0.50063215859030796</v>
       </c>
-      <c r="E29" s="83">
+      <c r="E29" s="74">
         <v>0.96293171806167399</v>
       </c>
       <c r="F29" s="16">
         <v>0.92096916299559495</v>
       </c>
-      <c r="G29" s="83">
+      <c r="G29" s="74">
         <v>0.96501762114537504</v>
       </c>
-      <c r="H29" s="83">
+      <c r="H29" s="74">
         <v>0.96302863436123398</v>
       </c>
-      <c r="I29" s="83">
+      <c r="I29" s="74">
         <v>0.96394493392070502</v>
       </c>
       <c r="J29" s="16">
         <v>0.60991850220264299</v>
       </c>
-      <c r="K29" s="84">
+      <c r="K29" s="75">
         <v>0.96231057268722497</v>
       </c>
     </row>
@@ -2900,7 +2900,7 @@
       <c r="D30" s="63">
         <v>0.79698678414096902</v>
       </c>
-      <c r="E30" s="79">
+      <c r="E30" s="70">
         <v>0.96119823788546199</v>
       </c>
       <c r="F30" s="64">
@@ -2909,16 +2909,16 @@
       <c r="G30" s="64">
         <v>0.95939647577092502</v>
       </c>
-      <c r="H30" s="79">
+      <c r="H30" s="70">
         <v>0.96497356828193903</v>
       </c>
-      <c r="I30" s="79">
+      <c r="I30" s="70">
         <v>0.96355947136563902</v>
       </c>
       <c r="J30" s="64">
         <v>0.68564096916299599</v>
       </c>
-      <c r="K30" s="80">
+      <c r="K30" s="71">
         <v>0.96677753303964797</v>
       </c>
     </row>
@@ -3100,61 +3100,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="74"/>
-      <c r="F3" s="73" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="73" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="73" t="s">
+      <c r="I3" s="82"/>
+      <c r="J3" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="74"/>
-      <c r="L3" s="73" t="s">
+      <c r="K3" s="82"/>
+      <c r="L3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="74"/>
-      <c r="N3" s="73" t="s">
+      <c r="M3" s="82"/>
+      <c r="N3" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="74"/>
-      <c r="P3" s="73" t="s">
+      <c r="O3" s="82"/>
+      <c r="P3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="73" t="s">
+      <c r="Q3" s="82"/>
+      <c r="R3" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="75"/>
+      <c r="S3" s="83"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -4440,19 +4440,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -5206,19 +5206,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -5976,32 +5976,32 @@
   <sheetData>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="71"/>
-      <c r="M3" s="69" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="79"/>
+      <c r="M3" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="71"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="79"/>
     </row>
     <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -7337,19 +7337,19 @@
     </row>
     <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M22" s="69" t="s">
+      <c r="M22" s="77" t="s">
         <v>319</v>
       </c>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="70"/>
-      <c r="S22" s="70"/>
-      <c r="T22" s="70"/>
-      <c r="U22" s="70"/>
-      <c r="V22" s="70"/>
-      <c r="W22" s="71"/>
+      <c r="N22" s="78"/>
+      <c r="O22" s="78"/>
+      <c r="P22" s="78"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="78"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="78"/>
+      <c r="W22" s="79"/>
     </row>
     <row r="23" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M23" s="2" t="s">
@@ -8067,19 +8067,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9191,19 +9191,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10118,19 +10118,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11095,8 +11095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D980D9F8-6B96-4F95-8395-B1BF7462FEB8}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11110,19 +11110,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12146,7 +12146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D696DEA4-1C6D-43BD-8BC6-2C617DFECF13}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -12159,19 +12159,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13195,8 +13195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40056-F547-48DD-9331-37B657810592}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13214,19 +13214,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14269,19 +14269,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15329,24 +15329,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15356,29 +15356,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="73" t="s">
+      <c r="K3" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="74"/>
-      <c r="M3" s="73" t="s">
+      <c r="L3" s="82"/>
+      <c r="M3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="73" t="s">
+      <c r="N3" s="82"/>
+      <c r="O3" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="75"/>
+      <c r="P3" s="83"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">

</xml_diff>